<commit_message>
Signed-off-by: Andres Rodriguez <a01287002@tec.mx>
</commit_message>
<xml_diff>
--- a/Segundo Parcial/assignment-14/db/registro.xlsx
+++ b/Segundo Parcial/assignment-14/db/registro.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\Programacion Prepa\Segundo Parcial\assignment-14\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1F4D32-DEB5-4A05-ACD3-453D30098891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E6C369-80EC-4BDB-A5F8-7D08BD78D37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID de transaccion</t>
   </si>
@@ -43,6 +54,18 @@
   </si>
   <si>
     <t>Operación</t>
+  </si>
+  <si>
+    <t>Reservar</t>
+  </si>
+  <si>
+    <t>Steve Jobs</t>
+  </si>
+  <si>
+    <t>Walter Issacson</t>
+  </si>
+  <si>
+    <t>Biography</t>
   </si>
 </sst>
 </file>
@@ -78,8 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,24 +384,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="1" customWidth="1"/>
+    <col min="3" max="6" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
@@ -391,9 +415,30 @@
       </c>
       <c r="F1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45735.926911689814</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>